<commit_message>
Fixed sync of different markets
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/my-repos/portfolio-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CA2FE9-A58B-914E-9838-EF34A5928C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D53F063-B1A6-904C-874D-E8F0ECE8574D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{27253425-B5D6-6E4C-B407-E0BACA28F10B}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,18 +41,6 @@
     <t>Tickers</t>
   </si>
   <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>AMZN</t>
-  </si>
-  <si>
-    <t>DPZ</t>
-  </si>
-  <si>
     <t>Weights</t>
   </si>
   <si>
@@ -74,6 +63,18 @@
   </si>
   <si>
     <t>UpperBound</t>
+  </si>
+  <si>
+    <t>SAN</t>
+  </si>
+  <si>
+    <t>REPYY</t>
+  </si>
+  <si>
+    <t>SLR.MC</t>
+  </si>
+  <si>
+    <t>MT</t>
   </si>
 </sst>
 </file>
@@ -140,71 +141,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -521,7 +462,7 @@
   <dimension ref="B3:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,59 +477,59 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
         <v>0.25</v>
       </c>
       <c r="H4" s="3">
-        <v>41275</v>
+        <v>42795</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <v>0.25</v>
@@ -597,7 +538,7 @@
     </row>
     <row r="6" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>0.25</v>
@@ -606,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
         <v>0.25</v>
@@ -615,16 +556,16 @@
     </row>
     <row r="7" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E7" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
         <v>0.25</v>
@@ -641,6 +582,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -671,17 +613,17 @@
   <sheetData>
     <row r="3" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>